<commit_message>
download data user and download data jawaban uraian siswa
</commit_message>
<xml_diff>
--- a/public/be_assets/exam/tempImportExam.xlsx
+++ b/public/be_assets/exam/tempImportExam.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t xml:space="preserve">TEMPLATE UJIAN URAIAN
 </t>
@@ -36,7 +36,10 @@
     <t xml:space="preserve">soal tanpa gmbr no 3 test soal soal soal </t>
   </si>
   <si>
-    <t>be_assets\exam\exam_d66b5eaa-3e22-4e05-80c2-09ff0a444609.png</t>
+    <t>be_assets\exam\exam_abd4e26f-5c1b-4da4-8dc9-e34a2f37efd0.png</t>
+  </si>
+  <si>
+    <t>be_assets\exam\exam_fffa81df-a25e-473a-8434-7cc0ab07d550.png</t>
   </si>
 </sst>
 </file>
@@ -136,6 +139,43 @@
       <xdr:spPr>
         <a:xfrm rot="0">
           <a:ext cx="2162175" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2676525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1571625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0">
+          <a:ext cx="2628900" cy="1504950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -437,10 +477,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A4">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -507,6 +547,14 @@
       </c>
       <c r="B10" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" customHeight="1" ht="129.75">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>